<commit_message>
Update the BOM and parts list.
</commit_message>
<xml_diff>
--- a/bom_partlist/sigma_mix_bom.xlsx
+++ b/bom_partlist/sigma_mix_bom.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18201"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18229"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shun\eagle\FXF\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shun\Desktop\CurrentProjects\SigmaMIX\SigmaMIX_Hardware\bom_partlist\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,12 +14,12 @@
   <sheets>
     <sheet name="partslist" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="717" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="703" uniqueCount="287">
   <si>
     <t>Part</t>
   </si>
@@ -567,10 +567,6 @@
   </si>
   <si>
     <t>SMD</t>
-    <phoneticPr fontId="18"/>
-  </si>
-  <si>
-    <t>535-10902-1-ND</t>
     <phoneticPr fontId="18"/>
   </si>
   <si>
@@ -694,293 +690,305 @@
     <t>CP-1420-ND</t>
   </si>
   <si>
+    <t>CP-1419-ND</t>
+  </si>
+  <si>
+    <t>Audio Connector</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>Audio Connector</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>Through Hole</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>2x5</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>2x6</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>2x6</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>Pin Header</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>BGM113</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>LGA Module</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>DC_JACK</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>Power Connector</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>Bluetooth Module</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>336-3817-1-ND</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>GREEN</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>RED</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>67-1002-1-ND</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>LED</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>67-1003-1-ND</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>600ohm@100MHz</t>
+  </si>
+  <si>
+    <t>490-14396-1-ND</t>
+  </si>
+  <si>
+    <t>490-14396-1-ND</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>Ferrite Beads</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>Ferrite Beads</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>1608</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>1608</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>1608</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>1608</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>2012</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>2012</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>2012</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>P49.9KHCT-ND</t>
+  </si>
+  <si>
+    <t>P56.2HCT-ND</t>
+  </si>
+  <si>
+    <t>P49.9KHCT-ND</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>P10.0KHCT-ND</t>
+  </si>
+  <si>
+    <t>P18.0KHCT-ND</t>
+  </si>
+  <si>
+    <t>P1.00KHCT-ND</t>
+  </si>
+  <si>
+    <t>P0.0ACT-ND</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>P100KHCT-ND</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>P475HCT-ND</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>P49.9KHCT-ND</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>P8.06KHCT-ND</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>P8.06KHCT-ND</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>P475HCT-ND</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>P562HCT-ND</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>Resistor</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>Resistor</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>Resistor</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t xml:space="preserve">490-1683-6-ND </t>
+  </si>
+  <si>
+    <t>Multilayer Ceramic Capacitor</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>Multilayer Ceramic Capacitor</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>Multilayer Ceramic Capacitor</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>Multilayer Ceramic Capacitor</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>Multilayer Ceramic Capacitor</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t xml:space="preserve">490-1662-1-ND </t>
+  </si>
+  <si>
+    <t>490-1615-1-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">399-1153-1-ND </t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>Multilayer Ceramic Capacitor</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>490-3905-1-ND</t>
+  </si>
+  <si>
+    <t>490-3905-1-ND</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>490-3905-1-ND</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>490-3905-1-ND</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>718-1313-1-ND</t>
+  </si>
+  <si>
+    <t>Tantalum Capacitor</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>Tantalum Capacitor</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>Tantalum Capacitor</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>3528</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>3528</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>3528</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>478-8115-1-ND</t>
+  </si>
+  <si>
+    <t>478-8115-1-ND</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>Tantalum Capacitor</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>Tantalum Capacitor</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>2012</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t xml:space="preserve">490-1691-1-ND </t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
     <t>CP-1420-ND</t>
     <phoneticPr fontId="18"/>
   </si>
   <si>
-    <t>CP-1419-ND</t>
-  </si>
-  <si>
-    <t>Audio Connector</t>
-    <phoneticPr fontId="18"/>
-  </si>
-  <si>
-    <t>Audio Connector</t>
-    <phoneticPr fontId="18"/>
-  </si>
-  <si>
-    <t>Through Hole</t>
-    <phoneticPr fontId="18"/>
-  </si>
-  <si>
-    <t>2x5</t>
-    <phoneticPr fontId="18"/>
-  </si>
-  <si>
-    <t>2x6</t>
-    <phoneticPr fontId="18"/>
-  </si>
-  <si>
-    <t>2x6</t>
-    <phoneticPr fontId="18"/>
-  </si>
-  <si>
-    <t>Pin Header</t>
-    <phoneticPr fontId="18"/>
-  </si>
-  <si>
-    <t>BGM113</t>
-    <phoneticPr fontId="18"/>
-  </si>
-  <si>
-    <t>LGA Module</t>
-    <phoneticPr fontId="18"/>
-  </si>
-  <si>
-    <t>DC_JACK</t>
-    <phoneticPr fontId="18"/>
-  </si>
-  <si>
-    <t>Power Connector</t>
-    <phoneticPr fontId="18"/>
-  </si>
-  <si>
-    <t>Bluetooth Module</t>
-    <phoneticPr fontId="18"/>
-  </si>
-  <si>
-    <t>336-3817-1-ND</t>
-    <phoneticPr fontId="18"/>
-  </si>
-  <si>
-    <t>GREEN</t>
-    <phoneticPr fontId="18"/>
-  </si>
-  <si>
-    <t>RED</t>
-    <phoneticPr fontId="18"/>
-  </si>
-  <si>
-    <t>67-1002-1-ND</t>
-    <phoneticPr fontId="18"/>
-  </si>
-  <si>
-    <t>LED</t>
-    <phoneticPr fontId="18"/>
-  </si>
-  <si>
-    <t>67-1003-1-ND</t>
-    <phoneticPr fontId="18"/>
-  </si>
-  <si>
-    <t>600ohm@100MHz</t>
-  </si>
-  <si>
-    <t>490-14396-1-ND</t>
-  </si>
-  <si>
-    <t>490-14396-1-ND</t>
-    <phoneticPr fontId="18"/>
-  </si>
-  <si>
-    <t>Ferrite Beads</t>
-    <phoneticPr fontId="18"/>
-  </si>
-  <si>
-    <t>Ferrite Beads</t>
-    <phoneticPr fontId="18"/>
-  </si>
-  <si>
-    <t>1608</t>
-    <phoneticPr fontId="18"/>
-  </si>
-  <si>
-    <t>1608</t>
-    <phoneticPr fontId="18"/>
-  </si>
-  <si>
-    <t>1608</t>
-    <phoneticPr fontId="18"/>
-  </si>
-  <si>
-    <t>1608</t>
-    <phoneticPr fontId="18"/>
-  </si>
-  <si>
-    <t>2012</t>
-    <phoneticPr fontId="18"/>
-  </si>
-  <si>
-    <t>2012</t>
-    <phoneticPr fontId="18"/>
-  </si>
-  <si>
-    <t>2012</t>
-    <phoneticPr fontId="18"/>
-  </si>
-  <si>
-    <t>P49.9KHCT-ND</t>
-  </si>
-  <si>
-    <t>P56.2HCT-ND</t>
-  </si>
-  <si>
-    <t>P49.9KHCT-ND</t>
-    <phoneticPr fontId="18"/>
-  </si>
-  <si>
-    <t>P10.0KHCT-ND</t>
-  </si>
-  <si>
-    <t>P18.0KHCT-ND</t>
-  </si>
-  <si>
-    <t>P1.00KHCT-ND</t>
-  </si>
-  <si>
-    <t>P0.0ACT-ND</t>
-    <phoneticPr fontId="18"/>
-  </si>
-  <si>
-    <t>P100KHCT-ND</t>
-    <phoneticPr fontId="18"/>
-  </si>
-  <si>
-    <t>P475HCT-ND</t>
-    <phoneticPr fontId="18"/>
-  </si>
-  <si>
-    <t>P49.9KHCT-ND</t>
-    <phoneticPr fontId="18"/>
-  </si>
-  <si>
-    <t>P8.06KHCT-ND</t>
-    <phoneticPr fontId="18"/>
-  </si>
-  <si>
-    <t>P8.06KHCT-ND</t>
-    <phoneticPr fontId="18"/>
-  </si>
-  <si>
-    <t>P475HCT-ND</t>
-    <phoneticPr fontId="18"/>
-  </si>
-  <si>
-    <t>P562HCT-ND</t>
-    <phoneticPr fontId="18"/>
-  </si>
-  <si>
-    <t>Resistor</t>
-    <phoneticPr fontId="18"/>
-  </si>
-  <si>
-    <t>Resistor</t>
-    <phoneticPr fontId="18"/>
-  </si>
-  <si>
-    <t>Resistor</t>
-    <phoneticPr fontId="18"/>
-  </si>
-  <si>
-    <t xml:space="preserve">490-1683-6-ND </t>
-  </si>
-  <si>
-    <t>Multilayer Ceramic Capacitor</t>
-    <phoneticPr fontId="18"/>
-  </si>
-  <si>
-    <t>Multilayer Ceramic Capacitor</t>
-    <phoneticPr fontId="18"/>
-  </si>
-  <si>
-    <t>Multilayer Ceramic Capacitor</t>
-    <phoneticPr fontId="18"/>
-  </si>
-  <si>
-    <t>Multilayer Ceramic Capacitor</t>
-    <phoneticPr fontId="18"/>
-  </si>
-  <si>
-    <t>Multilayer Ceramic Capacitor</t>
-    <phoneticPr fontId="18"/>
-  </si>
-  <si>
-    <t xml:space="preserve">490-1662-1-ND </t>
-  </si>
-  <si>
-    <t>490-1615-1-ND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">399-1153-1-ND </t>
-    <phoneticPr fontId="18"/>
-  </si>
-  <si>
-    <t>Multilayer Ceramic Capacitor</t>
-    <phoneticPr fontId="18"/>
-  </si>
-  <si>
-    <t>490-3905-1-ND</t>
-  </si>
-  <si>
-    <t>490-3905-1-ND</t>
-    <phoneticPr fontId="18"/>
-  </si>
-  <si>
-    <t>490-3905-1-ND</t>
-    <phoneticPr fontId="18"/>
-  </si>
-  <si>
-    <t>490-3905-1-ND</t>
-    <phoneticPr fontId="18"/>
-  </si>
-  <si>
-    <t>718-1313-1-ND</t>
-  </si>
-  <si>
-    <t>Tantalum Capacitor</t>
-    <phoneticPr fontId="18"/>
-  </si>
-  <si>
-    <t>Tantalum Capacitor</t>
-    <phoneticPr fontId="18"/>
-  </si>
-  <si>
-    <t>Tantalum Capacitor</t>
-    <phoneticPr fontId="18"/>
-  </si>
-  <si>
-    <t>3528</t>
-    <phoneticPr fontId="18"/>
-  </si>
-  <si>
-    <t>3528</t>
-    <phoneticPr fontId="18"/>
-  </si>
-  <si>
-    <t>3528</t>
-    <phoneticPr fontId="18"/>
-  </si>
-  <si>
-    <t>478-8115-1-ND</t>
-  </si>
-  <si>
-    <t>478-8115-1-ND</t>
-    <phoneticPr fontId="18"/>
-  </si>
-  <si>
-    <t>Tantalum Capacitor</t>
-    <phoneticPr fontId="18"/>
-  </si>
-  <si>
-    <t>Tantalum Capacitor</t>
-    <phoneticPr fontId="18"/>
-  </si>
-  <si>
-    <t>2012</t>
-    <phoneticPr fontId="18"/>
-  </si>
-  <si>
-    <t xml:space="preserve">490-1691-1-ND </t>
+    <t>SC1313-ND</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t xml:space="preserve">SW426-ND </t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>SER4107CT-ND</t>
     <phoneticPr fontId="18"/>
   </si>
 </sst>
@@ -988,7 +996,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1168,6 +1176,13 @@
       <color rgb="FF000000"/>
       <name val="游ゴシック"/>
       <family val="3"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="游ゴシック"/>
+      <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
     </font>
@@ -1636,7 +1651,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1680,6 +1695,9 @@
       <alignment vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" shrinkToFit="1"/>
     </xf>
   </cellXfs>
@@ -2047,8 +2065,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F142"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D142"/>
+    <sheetView tabSelected="1" topLeftCell="A127" workbookViewId="0">
+      <selection activeCell="M139" sqref="M139"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -2086,13 +2104,13 @@
         <v>4</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="F2" s="1"/>
     </row>
@@ -2104,13 +2122,13 @@
         <v>6</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="F3" s="1"/>
     </row>
@@ -2122,13 +2140,13 @@
         <v>8</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="F4" s="1"/>
     </row>
@@ -2140,13 +2158,13 @@
         <v>8</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="F5" s="1"/>
     </row>
@@ -2158,13 +2176,13 @@
         <v>8</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="F6" s="1"/>
     </row>
@@ -2176,13 +2194,13 @@
         <v>6</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="F7" s="1"/>
     </row>
@@ -2194,13 +2212,13 @@
         <v>8</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="F8" s="1"/>
     </row>
@@ -2212,13 +2230,13 @@
         <v>8</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="F9" s="1"/>
     </row>
@@ -2230,13 +2248,13 @@
         <v>15</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="F10" s="1"/>
     </row>
@@ -2248,13 +2266,13 @@
         <v>6</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="F11" s="1"/>
     </row>
@@ -2266,13 +2284,13 @@
         <v>6</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="F12" s="1"/>
     </row>
@@ -2284,13 +2302,13 @@
         <v>8</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="F13" s="1"/>
     </row>
@@ -2302,13 +2320,13 @@
         <v>8</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="F14" s="1"/>
     </row>
@@ -2320,13 +2338,13 @@
         <v>8</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="E15" s="9" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="F15" s="1"/>
     </row>
@@ -2338,13 +2356,13 @@
         <v>6</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="E16" s="9" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="F16" s="1"/>
     </row>
@@ -2356,13 +2374,13 @@
         <v>8</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="F17" s="1"/>
     </row>
@@ -2374,13 +2392,13 @@
         <v>8</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="E18" s="9" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="F18" s="1"/>
     </row>
@@ -2392,13 +2410,13 @@
         <v>6</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="E19" s="9" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="F19" s="1"/>
     </row>
@@ -2410,13 +2428,13 @@
         <v>8</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="E20" s="9" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="F20" s="1"/>
     </row>
@@ -2428,13 +2446,13 @@
         <v>6</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="E21" s="9" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="F21" s="1"/>
     </row>
@@ -2446,13 +2464,13 @@
         <v>8</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="E22" s="9" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="F22" s="1"/>
     </row>
@@ -2464,13 +2482,13 @@
         <v>6</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="E23" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="F23" s="1"/>
     </row>
@@ -2482,13 +2500,13 @@
         <v>15</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E24" s="9" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="F24" s="1"/>
     </row>
@@ -2500,13 +2518,13 @@
         <v>31</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="E25" s="9" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="F25" s="1"/>
     </row>
@@ -2518,13 +2536,13 @@
         <v>33</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="E26" s="9" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="F26" s="1"/>
     </row>
@@ -2536,13 +2554,13 @@
         <v>6</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="E27" s="9" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="F27" s="1"/>
     </row>
@@ -2554,13 +2572,13 @@
         <v>36</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="D28" s="9" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="E28" s="9" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="F28" s="1"/>
     </row>
@@ -2572,13 +2590,13 @@
         <v>36</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="D29" s="9" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="E29" s="9" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="F29" s="1"/>
     </row>
@@ -2590,13 +2608,13 @@
         <v>15</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E30" s="9" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="F30" s="1"/>
     </row>
@@ -2608,13 +2626,13 @@
         <v>15</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="D31" s="9" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E31" s="9" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="F31" s="1"/>
     </row>
@@ -2626,13 +2644,13 @@
         <v>31</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="D32" s="9" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="E32" s="9" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="F32" s="1"/>
     </row>
@@ -2644,13 +2662,13 @@
         <v>31</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="D33" s="9" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="E33" s="9" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="F33" s="1"/>
     </row>
@@ -2662,13 +2680,13 @@
         <v>31</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="D34" s="9" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="E34" s="9" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="F34" s="1"/>
     </row>
@@ -2680,13 +2698,13 @@
         <v>31</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="D35" s="9" t="s">
+        <v>260</v>
+      </c>
+      <c r="E35" s="9" t="s">
         <v>262</v>
-      </c>
-      <c r="E35" s="9" t="s">
-        <v>264</v>
       </c>
       <c r="F35" s="1"/>
     </row>
@@ -2698,13 +2716,13 @@
         <v>8</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="D36" s="9" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="E36" s="9" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="F36" s="1"/>
     </row>
@@ -2716,13 +2734,13 @@
         <v>8</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="D37" s="9" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="E37" s="9" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="F37" s="1"/>
     </row>
@@ -2734,13 +2752,13 @@
         <v>6</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="D38" s="9" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="E38" s="9" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="F38" s="1"/>
     </row>
@@ -2752,13 +2770,13 @@
         <v>8</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="D39" s="9" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="E39" s="9" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="F39" s="1"/>
     </row>
@@ -2770,13 +2788,13 @@
         <v>15</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="D40" s="9" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="E40" s="9" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="F40" s="1"/>
     </row>
@@ -2788,13 +2806,13 @@
         <v>6</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="D41" s="9" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="E41" s="9" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="F41" s="1"/>
     </row>
@@ -2806,13 +2824,13 @@
         <v>6</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="D42" s="9" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="E42" s="9" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="F42" s="1"/>
     </row>
@@ -2824,13 +2842,13 @@
         <v>8</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D43" s="9" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="E43" s="9" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="F43" s="1"/>
     </row>
@@ -2842,13 +2860,13 @@
         <v>8</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="D44" s="9" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="E44" s="9" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="F44" s="1"/>
     </row>
@@ -2860,13 +2878,13 @@
         <v>8</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="D45" s="9" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="E45" s="9" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="F45" s="1"/>
     </row>
@@ -2878,13 +2896,13 @@
         <v>6</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="D46" s="9" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="E46" s="9" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="F46" s="1"/>
     </row>
@@ -2896,13 +2914,13 @@
         <v>8</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="D47" s="9" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="E47" s="9" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="F47" s="1"/>
     </row>
@@ -2914,13 +2932,13 @@
         <v>8</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="D48" s="9" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="E48" s="9" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="F48" s="1"/>
     </row>
@@ -2932,13 +2950,13 @@
         <v>6</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="D49" s="9" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="E49" s="9" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F49" s="1"/>
     </row>
@@ -2950,13 +2968,13 @@
         <v>8</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="D50" s="9" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="E50" s="9" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="F50" s="1"/>
     </row>
@@ -2968,13 +2986,13 @@
         <v>6</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="D51" s="9" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="E51" s="9" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="F51" s="1"/>
     </row>
@@ -2986,13 +3004,13 @@
         <v>8</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D52" s="9" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="E52" s="9" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="F52" s="1"/>
     </row>
@@ -3004,13 +3022,13 @@
         <v>6</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="D53" s="9" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="E53" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="F53" s="1"/>
     </row>
@@ -3022,13 +3040,13 @@
         <v>15</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="D54" s="9" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E54" s="9" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="F54" s="1"/>
     </row>
@@ -3040,13 +3058,13 @@
         <v>31</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D55" s="9" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="E55" s="9" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="F55" s="1"/>
     </row>
@@ -3058,13 +3076,13 @@
         <v>33</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="D56" s="9" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="E56" s="9" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="F56" s="1"/>
     </row>
@@ -3076,13 +3094,13 @@
         <v>6</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D57" s="9" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="E57" s="9" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="F57" s="1"/>
     </row>
@@ -3094,13 +3112,13 @@
         <v>36</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="D58" s="9" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="E58" s="9" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="F58" s="1"/>
     </row>
@@ -3112,13 +3130,13 @@
         <v>36</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="D59" s="9" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="E59" s="9" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="F59" s="1"/>
     </row>
@@ -3130,13 +3148,13 @@
         <v>15</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="D60" s="9" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E60" s="9" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="F60" s="1"/>
     </row>
@@ -3148,13 +3166,13 @@
         <v>15</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="D61" s="9" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="E61" s="9" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="F61" s="1"/>
     </row>
@@ -3166,13 +3184,13 @@
         <v>31</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="D62" s="9" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="E62" s="9" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="F62" s="1"/>
     </row>
@@ -3184,13 +3202,13 @@
         <v>31</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="D63" s="9" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="E63" s="9" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="F63" s="1"/>
     </row>
@@ -3202,13 +3220,13 @@
         <v>31</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="D64" s="9" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="E64" s="9" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="F64" s="1"/>
     </row>
@@ -3220,13 +3238,13 @@
         <v>31</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="D65" s="9" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="E65" s="9" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="F65" s="1"/>
     </row>
@@ -3235,16 +3253,16 @@
         <v>74</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="D66" s="9" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="E66" s="9" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="F66" s="1"/>
     </row>
@@ -3253,195 +3271,179 @@
         <v>75</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C67" s="2" t="s">
         <v>167</v>
       </c>
       <c r="D67" s="9" t="s">
-        <v>221</v>
-      </c>
-      <c r="E67" s="10"/>
-      <c r="F67" s="3" t="s">
-        <v>187</v>
-      </c>
+        <v>219</v>
+      </c>
+      <c r="E67" s="15" t="s">
+        <v>284</v>
+      </c>
+      <c r="F67" s="3"/>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A68" s="1" t="s">
         <v>76</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C68" s="2" t="s">
         <v>167</v>
       </c>
       <c r="D68" s="9" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="E68" s="9" t="s">
-        <v>207</v>
-      </c>
-      <c r="F68" s="4" t="s">
-        <v>187</v>
-      </c>
+        <v>206</v>
+      </c>
+      <c r="F68" s="4"/>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A69" s="1" t="s">
         <v>77</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D69" s="9" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="E69" s="9" t="s">
-        <v>210</v>
-      </c>
-      <c r="F69" s="4" t="s">
-        <v>187</v>
-      </c>
+        <v>208</v>
+      </c>
+      <c r="F69" s="4"/>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A70" s="1" t="s">
         <v>78</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C70" s="2" t="s">
         <v>167</v>
       </c>
       <c r="D70" s="9" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="E70" s="9" t="s">
-        <v>209</v>
-      </c>
-      <c r="F70" s="4" t="s">
-        <v>187</v>
-      </c>
+        <v>283</v>
+      </c>
+      <c r="F70" s="4"/>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A71" s="1" t="s">
         <v>79</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C71" s="2" t="s">
         <v>167</v>
       </c>
       <c r="D71" s="9" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="E71" s="9" t="s">
-        <v>206</v>
-      </c>
-      <c r="F71" s="4" t="s">
-        <v>187</v>
-      </c>
+        <v>205</v>
+      </c>
+      <c r="F71" s="4"/>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A72" s="1" t="s">
         <v>80</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="D72" s="9" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="E72" s="9" t="s">
-        <v>206</v>
-      </c>
-      <c r="F72" s="4" t="s">
-        <v>187</v>
-      </c>
+        <v>205</v>
+      </c>
+      <c r="F72" s="4"/>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A73" s="1" t="s">
         <v>81</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D73" s="9" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="E73" s="9" t="s">
-        <v>210</v>
-      </c>
-      <c r="F73" s="4" t="s">
-        <v>187</v>
-      </c>
+        <v>208</v>
+      </c>
+      <c r="F73" s="4"/>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A74" s="1" t="s">
         <v>82</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C74" s="2" t="s">
         <v>167</v>
       </c>
       <c r="D74" s="9" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="E74" s="9" t="s">
-        <v>208</v>
-      </c>
-      <c r="F74" s="4" t="s">
-        <v>187</v>
-      </c>
+        <v>207</v>
+      </c>
+      <c r="F74" s="4"/>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A75" s="1" t="s">
         <v>83</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C75" s="2" t="s">
         <v>167</v>
       </c>
       <c r="D75" s="9" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="E75" s="9" t="s">
-        <v>207</v>
-      </c>
-      <c r="F75" s="4" t="s">
-        <v>187</v>
-      </c>
+        <v>206</v>
+      </c>
+      <c r="F75" s="4"/>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A76" s="1" t="s">
         <v>84</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C76" s="2" t="s">
         <v>167</v>
       </c>
       <c r="D76" s="9" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E76" s="10"/>
       <c r="F76" s="4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.4">
@@ -3449,17 +3451,17 @@
         <v>85</v>
       </c>
       <c r="B77" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="C77" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="D77" s="9" t="s">
         <v>215</v>
-      </c>
-      <c r="C77" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="D77" s="9" t="s">
-        <v>217</v>
       </c>
       <c r="E77" s="11"/>
       <c r="F77" s="4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.4">
@@ -3467,17 +3469,17 @@
         <v>86</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C78" s="2" t="s">
         <v>167</v>
       </c>
       <c r="D78" s="9" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E78" s="11"/>
       <c r="F78" s="4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.4">
@@ -3485,16 +3487,16 @@
         <v>87</v>
       </c>
       <c r="B79" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="C79" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="D79" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="E79" s="12" t="s">
         <v>229</v>
-      </c>
-      <c r="C79" s="2" t="s">
-        <v>234</v>
-      </c>
-      <c r="D79" s="9" t="s">
-        <v>232</v>
-      </c>
-      <c r="E79" s="12" t="s">
-        <v>231</v>
       </c>
       <c r="F79" s="1"/>
     </row>
@@ -3503,16 +3505,16 @@
         <v>88</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D80" s="9" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="E80" s="9" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="F80" s="1"/>
     </row>
@@ -3521,16 +3523,16 @@
         <v>89</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D81" s="9" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="E81" s="9" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="F81" s="1"/>
     </row>
@@ -3539,16 +3541,16 @@
         <v>90</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D82" s="9" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="E82" s="9" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="F82" s="1"/>
     </row>
@@ -3557,16 +3559,16 @@
         <v>91</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C83" s="2">
         <v>3216</v>
       </c>
       <c r="D83" s="9" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="E83" s="9" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="F83" s="1"/>
     </row>
@@ -3575,16 +3577,16 @@
         <v>92</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C84" s="2">
         <v>3216</v>
       </c>
       <c r="D84" s="9" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="E84" s="9" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="F84" s="1"/>
     </row>
@@ -3596,13 +3598,13 @@
         <v>94</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D85" s="9" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="E85" s="9" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="F85" s="1"/>
     </row>
@@ -3614,13 +3616,13 @@
         <v>562</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D86" s="9" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="E86" s="9" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F86" s="1"/>
     </row>
@@ -3632,13 +3634,13 @@
         <v>97</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D87" s="9" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="E87" s="9" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="F87" s="1"/>
     </row>
@@ -3650,13 +3652,13 @@
         <v>99</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D88" s="9" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="E88" s="9" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="F88" s="1"/>
     </row>
@@ -3668,13 +3670,13 @@
         <v>101</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D89" s="9" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="E89" s="9" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="F89" s="1"/>
     </row>
@@ -3686,13 +3688,13 @@
         <v>103</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D90" s="9" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="E90" s="9" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="F90" s="1"/>
     </row>
@@ -3704,13 +3706,13 @@
         <v>101</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D91" s="9" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="E91" s="9" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="F91" s="1"/>
     </row>
@@ -3722,13 +3724,13 @@
         <v>103</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D92" s="9" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="E92" s="13" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="F92" s="1"/>
     </row>
@@ -3740,13 +3742,13 @@
         <v>101</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D93" s="9" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="E93" s="9" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="F93" s="1"/>
     </row>
@@ -3758,13 +3760,13 @@
         <v>108</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D94" s="9" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="E94" s="9" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="F94" s="1"/>
     </row>
@@ -3776,13 +3778,13 @@
         <v>108</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D95" s="9" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="E95" s="9" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="F95" s="1"/>
     </row>
@@ -3794,13 +3796,13 @@
         <v>111</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D96" s="9" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="E96" s="9" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="F96" s="1"/>
     </row>
@@ -3812,13 +3814,13 @@
         <v>475</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D97" s="9" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="E97" s="9" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="F97" s="1"/>
     </row>
@@ -3830,13 +3832,13 @@
         <v>101</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D98" s="9" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="E98" s="9" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="F98" s="1"/>
     </row>
@@ -3848,13 +3850,13 @@
         <v>108</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D99" s="9" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="E99" s="9" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="F99" s="1"/>
     </row>
@@ -3866,13 +3868,13 @@
         <v>108</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D100" s="9" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="E100" s="9" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="F100" s="1"/>
     </row>
@@ -3884,13 +3886,13 @@
         <v>108</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D101" s="9" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="E101" s="9" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="F101" s="1"/>
     </row>
@@ -3902,13 +3904,13 @@
         <v>108</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D102" s="9" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="E102" s="9" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="F102" s="1"/>
     </row>
@@ -3920,13 +3922,13 @@
         <v>99</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D103" s="9" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="E103" s="9" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="F103" s="1"/>
     </row>
@@ -3938,13 +3940,13 @@
         <v>99</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="D104" s="9" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="E104" s="9" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="F104" s="1"/>
     </row>
@@ -3956,13 +3958,13 @@
         <v>99</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D105" s="9" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="E105" s="9" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="F105" s="1"/>
     </row>
@@ -3974,13 +3976,13 @@
         <v>99</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D106" s="9" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="E106" s="9" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="F106" s="1"/>
     </row>
@@ -3992,13 +3994,13 @@
         <v>0</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D107" s="9" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="E107" s="9" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="F107" s="1"/>
     </row>
@@ -4010,13 +4012,13 @@
         <v>97</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D108" s="9" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="E108" s="9" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="F108" s="1"/>
     </row>
@@ -4028,13 +4030,13 @@
         <v>101</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D109" s="9" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="E109" s="9" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="F109" s="1"/>
     </row>
@@ -4046,13 +4048,13 @@
         <v>103</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D110" s="9" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="E110" s="9" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="F110" s="1"/>
     </row>
@@ -4064,13 +4066,13 @@
         <v>101</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D111" s="9" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="E111" s="9" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="F111" s="1"/>
     </row>
@@ -4082,13 +4084,13 @@
         <v>103</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D112" s="9" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="E112" s="9" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="F112" s="1"/>
     </row>
@@ -4100,13 +4102,13 @@
         <v>101</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D113" s="9" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="E113" s="9" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="F113" s="1"/>
     </row>
@@ -4118,13 +4120,13 @@
         <v>108</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="D114" s="9" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="E114" s="9" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="F114" s="1"/>
     </row>
@@ -4136,13 +4138,13 @@
         <v>108</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D115" s="9" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="E115" s="9" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="F115" s="1"/>
     </row>
@@ -4154,13 +4156,13 @@
         <v>111</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D116" s="9" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="E116" s="9" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="F116" s="1"/>
     </row>
@@ -4172,13 +4174,13 @@
         <v>475</v>
       </c>
       <c r="C117" s="2" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D117" s="9" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="E117" s="9" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="F117" s="1"/>
     </row>
@@ -4190,13 +4192,13 @@
         <v>101</v>
       </c>
       <c r="C118" s="2" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D118" s="9" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="E118" s="9" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="F118" s="1"/>
     </row>
@@ -4208,13 +4210,13 @@
         <v>108</v>
       </c>
       <c r="C119" s="2" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D119" s="9" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="E119" s="9" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="F119" s="1"/>
     </row>
@@ -4226,13 +4228,13 @@
         <v>108</v>
       </c>
       <c r="C120" s="2" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D120" s="9" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="E120" s="9" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="F120" s="1"/>
     </row>
@@ -4244,13 +4246,13 @@
         <v>108</v>
       </c>
       <c r="C121" s="2" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D121" s="9" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="E121" s="9" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="F121" s="1"/>
     </row>
@@ -4262,13 +4264,13 @@
         <v>108</v>
       </c>
       <c r="C122" s="2" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D122" s="9" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="E122" s="9" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="F122" s="1"/>
     </row>
@@ -4280,13 +4282,13 @@
         <v>99</v>
       </c>
       <c r="C123" s="2" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D123" s="9" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="E123" s="9" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="F123" s="1"/>
     </row>
@@ -4298,13 +4300,13 @@
         <v>99</v>
       </c>
       <c r="C124" s="2" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D124" s="9" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="E124" s="9" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="F124" s="1"/>
     </row>
@@ -4316,13 +4318,13 @@
         <v>99</v>
       </c>
       <c r="C125" s="2" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D125" s="9" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="E125" s="9" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="F125" s="1"/>
     </row>
@@ -4334,13 +4336,13 @@
         <v>99</v>
       </c>
       <c r="C126" s="2" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D126" s="9" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="E126" s="9" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="F126" s="1"/>
     </row>
@@ -4352,13 +4354,13 @@
         <v>562</v>
       </c>
       <c r="C127" s="2" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D127" s="9" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="E127" s="9" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F127" s="1"/>
     </row>
@@ -4378,9 +4380,7 @@
       <c r="E128" s="9" t="s">
         <v>172</v>
       </c>
-      <c r="F128" s="4" t="s">
-        <v>187</v>
-      </c>
+      <c r="F128" s="4"/>
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A129" s="1" t="s">
@@ -4396,28 +4396,26 @@
         <v>166</v>
       </c>
       <c r="E129" s="9" t="s">
-        <v>172</v>
-      </c>
-      <c r="F129" s="4" t="s">
-        <v>187</v>
-      </c>
+        <v>285</v>
+      </c>
+      <c r="F129" s="4"/>
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A130" s="1" t="s">
         <v>145</v>
       </c>
       <c r="B130" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C130" s="2" t="s">
         <v>167</v>
       </c>
       <c r="D130" s="9" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E130" s="10"/>
       <c r="F130" s="4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.4">
@@ -4425,17 +4423,17 @@
         <v>146</v>
       </c>
       <c r="B131" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C131" s="2" t="s">
         <v>167</v>
       </c>
       <c r="D131" s="9" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E131" s="11"/>
       <c r="F131" s="4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.4">
@@ -4454,9 +4452,7 @@
       <c r="E132" s="9" t="s">
         <v>168</v>
       </c>
-      <c r="F132" s="4" t="s">
-        <v>187</v>
-      </c>
+      <c r="F132" s="4"/>
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A133" s="1" t="s">
@@ -4474,9 +4470,7 @@
       <c r="E133" s="9" t="s">
         <v>169</v>
       </c>
-      <c r="F133" s="4" t="s">
-        <v>187</v>
-      </c>
+      <c r="F133" s="4"/>
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A134" s="1" t="s">
@@ -4519,16 +4513,16 @@
         <v>152</v>
       </c>
       <c r="B136" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C136" s="2" t="s">
         <v>153</v>
       </c>
       <c r="D136" s="9" t="s">
+        <v>188</v>
+      </c>
+      <c r="E136" s="9" t="s">
         <v>189</v>
-      </c>
-      <c r="E136" s="9" t="s">
-        <v>190</v>
       </c>
       <c r="F136" s="1"/>
     </row>
@@ -4537,16 +4531,16 @@
         <v>154</v>
       </c>
       <c r="B137" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="C137" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="C137" s="2" t="s">
+      <c r="D137" s="9" t="s">
         <v>192</v>
       </c>
-      <c r="D137" s="9" t="s">
+      <c r="E137" s="9" t="s">
         <v>193</v>
-      </c>
-      <c r="E137" s="9" t="s">
-        <v>194</v>
       </c>
       <c r="F137" s="1"/>
     </row>
@@ -4555,16 +4549,16 @@
         <v>155</v>
       </c>
       <c r="B138" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C138" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D138" s="9" t="s">
+        <v>198</v>
+      </c>
+      <c r="E138" s="9" t="s">
         <v>199</v>
-      </c>
-      <c r="E138" s="9" t="s">
-        <v>200</v>
       </c>
       <c r="F138" s="1"/>
     </row>
@@ -4573,16 +4567,16 @@
         <v>156</v>
       </c>
       <c r="B139" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C139" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="D139" s="9" t="s">
         <v>198</v>
       </c>
-      <c r="D139" s="9" t="s">
-        <v>199</v>
-      </c>
       <c r="E139" s="9" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F139" s="1"/>
     </row>
@@ -4591,20 +4585,18 @@
         <v>157</v>
       </c>
       <c r="B140" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C140" s="2" t="s">
         <v>167</v>
       </c>
       <c r="D140" s="9" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E140" s="9" t="s">
-        <v>182</v>
-      </c>
-      <c r="F140" s="3" t="s">
-        <v>187</v>
-      </c>
+        <v>181</v>
+      </c>
+      <c r="F140" s="3"/>
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A141" s="1" t="s">
@@ -4614,17 +4606,15 @@
         <v>159</v>
       </c>
       <c r="C141" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D141" s="9" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E141" s="9" t="s">
-        <v>183</v>
-      </c>
-      <c r="F141" s="4" t="s">
-        <v>187</v>
-      </c>
+        <v>182</v>
+      </c>
+      <c r="F141" s="4"/>
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A142" s="5" t="s">
@@ -4637,10 +4627,10 @@
         <v>177</v>
       </c>
       <c r="D142" s="14" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E142" s="14" t="s">
-        <v>178</v>
+        <v>286</v>
       </c>
       <c r="F142" s="5"/>
     </row>

</xml_diff>

<commit_message>
Revert "Update the BOM and parts list."
This reverts commit 2f607d859bf7c325c92fad7b5bdf895f4607e224.
</commit_message>
<xml_diff>
--- a/bom_partlist/sigma_mix_bom.xlsx
+++ b/bom_partlist/sigma_mix_bom.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18229"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18201"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shun\Desktop\CurrentProjects\SigmaMIX\SigmaMIX_Hardware\bom_partlist\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shun\eagle\FXF\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,12 +14,12 @@
   <sheets>
     <sheet name="partslist" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="703" uniqueCount="287">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="717" uniqueCount="285">
   <si>
     <t>Part</t>
   </si>
@@ -567,6 +567,10 @@
   </si>
   <si>
     <t>SMD</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>535-10902-1-ND</t>
     <phoneticPr fontId="18"/>
   </si>
   <si>
@@ -690,6 +694,10 @@
     <t>CP-1420-ND</t>
   </si>
   <si>
+    <t>CP-1420-ND</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
     <t>CP-1419-ND</t>
   </si>
   <si>
@@ -973,22 +981,6 @@
   </si>
   <si>
     <t xml:space="preserve">490-1691-1-ND </t>
-    <phoneticPr fontId="18"/>
-  </si>
-  <si>
-    <t>CP-1420-ND</t>
-    <phoneticPr fontId="18"/>
-  </si>
-  <si>
-    <t>SC1313-ND</t>
-    <phoneticPr fontId="18"/>
-  </si>
-  <si>
-    <t xml:space="preserve">SW426-ND </t>
-    <phoneticPr fontId="18"/>
-  </si>
-  <si>
-    <t>SER4107CT-ND</t>
     <phoneticPr fontId="18"/>
   </si>
 </sst>
@@ -996,7 +988,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="23" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1176,13 +1168,6 @@
       <color rgb="FF000000"/>
       <name val="游ゴシック"/>
       <family val="3"/>
-      <charset val="128"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="游ゴシック"/>
-      <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
     </font>
@@ -1651,7 +1636,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1695,9 +1680,6 @@
       <alignment vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" shrinkToFit="1"/>
     </xf>
   </cellXfs>
@@ -2065,8 +2047,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F142"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A127" workbookViewId="0">
-      <selection activeCell="M139" sqref="M139"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D142"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -2104,13 +2086,13 @@
         <v>4</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="F2" s="1"/>
     </row>
@@ -2122,13 +2104,13 @@
         <v>6</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="F3" s="1"/>
     </row>
@@ -2140,13 +2122,13 @@
         <v>8</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="F4" s="1"/>
     </row>
@@ -2158,13 +2140,13 @@
         <v>8</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="F5" s="1"/>
     </row>
@@ -2176,13 +2158,13 @@
         <v>8</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="D6" s="9" t="s">
+        <v>260</v>
+      </c>
+      <c r="E6" s="9" t="s">
         <v>258</v>
-      </c>
-      <c r="E6" s="9" t="s">
-        <v>256</v>
       </c>
       <c r="F6" s="1"/>
     </row>
@@ -2194,13 +2176,13 @@
         <v>6</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="F7" s="1"/>
     </row>
@@ -2212,13 +2194,13 @@
         <v>8</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="D8" s="9" t="s">
+        <v>260</v>
+      </c>
+      <c r="E8" s="9" t="s">
         <v>258</v>
-      </c>
-      <c r="E8" s="9" t="s">
-        <v>256</v>
       </c>
       <c r="F8" s="1"/>
     </row>
@@ -2230,13 +2212,13 @@
         <v>8</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="F9" s="1"/>
     </row>
@@ -2248,13 +2230,13 @@
         <v>15</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="F10" s="1"/>
     </row>
@@ -2266,13 +2248,13 @@
         <v>6</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="F11" s="1"/>
     </row>
@@ -2284,13 +2266,13 @@
         <v>6</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="F12" s="1"/>
     </row>
@@ -2302,13 +2284,13 @@
         <v>8</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="F13" s="1"/>
     </row>
@@ -2320,13 +2302,13 @@
         <v>8</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="D14" s="9" t="s">
+        <v>260</v>
+      </c>
+      <c r="E14" s="9" t="s">
         <v>258</v>
-      </c>
-      <c r="E14" s="9" t="s">
-        <v>256</v>
       </c>
       <c r="F14" s="1"/>
     </row>
@@ -2338,13 +2320,13 @@
         <v>8</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="D15" s="9" t="s">
+        <v>260</v>
+      </c>
+      <c r="E15" s="9" t="s">
         <v>258</v>
-      </c>
-      <c r="E15" s="9" t="s">
-        <v>256</v>
       </c>
       <c r="F15" s="1"/>
     </row>
@@ -2356,13 +2338,13 @@
         <v>6</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="D16" s="9" t="s">
+        <v>281</v>
+      </c>
+      <c r="E16" s="9" t="s">
         <v>279</v>
-      </c>
-      <c r="E16" s="9" t="s">
-        <v>277</v>
       </c>
       <c r="F16" s="1"/>
     </row>
@@ -2374,13 +2356,13 @@
         <v>8</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="F17" s="1"/>
     </row>
@@ -2392,13 +2374,13 @@
         <v>8</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="E18" s="9" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="F18" s="1"/>
     </row>
@@ -2410,13 +2392,13 @@
         <v>6</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="E19" s="9" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="F19" s="1"/>
     </row>
@@ -2428,13 +2410,13 @@
         <v>8</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="E20" s="9" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="F20" s="1"/>
     </row>
@@ -2446,13 +2428,13 @@
         <v>6</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="E21" s="9" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="F21" s="1"/>
     </row>
@@ -2464,13 +2446,13 @@
         <v>8</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="D22" s="9" t="s">
+        <v>260</v>
+      </c>
+      <c r="E22" s="9" t="s">
         <v>258</v>
-      </c>
-      <c r="E22" s="9" t="s">
-        <v>256</v>
       </c>
       <c r="F22" s="1"/>
     </row>
@@ -2482,13 +2464,13 @@
         <v>6</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="E23" s="9" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="F23" s="1"/>
     </row>
@@ -2500,13 +2482,13 @@
         <v>15</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="D24" s="9" t="s">
+        <v>274</v>
+      </c>
+      <c r="E24" s="9" t="s">
         <v>272</v>
-      </c>
-      <c r="E24" s="9" t="s">
-        <v>270</v>
       </c>
       <c r="F24" s="1"/>
     </row>
@@ -2518,13 +2500,13 @@
         <v>31</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="E25" s="9" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="F25" s="1"/>
     </row>
@@ -2536,13 +2518,13 @@
         <v>33</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="E26" s="9" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="F26" s="1"/>
     </row>
@@ -2554,13 +2536,13 @@
         <v>6</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="E27" s="9" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="F27" s="1"/>
     </row>
@@ -2572,13 +2554,13 @@
         <v>36</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="D28" s="9" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="E28" s="9" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="F28" s="1"/>
     </row>
@@ -2590,13 +2572,13 @@
         <v>36</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="D29" s="9" t="s">
+        <v>267</v>
+      </c>
+      <c r="E29" s="9" t="s">
         <v>265</v>
-      </c>
-      <c r="E29" s="9" t="s">
-        <v>263</v>
       </c>
       <c r="F29" s="1"/>
     </row>
@@ -2608,13 +2590,13 @@
         <v>15</v>
       </c>
       <c r="C30" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="D30" s="9" t="s">
         <v>274</v>
       </c>
-      <c r="D30" s="9" t="s">
+      <c r="E30" s="9" t="s">
         <v>272</v>
-      </c>
-      <c r="E30" s="9" t="s">
-        <v>270</v>
       </c>
       <c r="F30" s="1"/>
     </row>
@@ -2626,13 +2608,13 @@
         <v>15</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="D31" s="9" t="s">
+        <v>274</v>
+      </c>
+      <c r="E31" s="9" t="s">
         <v>272</v>
-      </c>
-      <c r="E31" s="9" t="s">
-        <v>270</v>
       </c>
       <c r="F31" s="1"/>
     </row>
@@ -2644,13 +2626,13 @@
         <v>31</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="D32" s="9" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="E32" s="9" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="F32" s="1"/>
     </row>
@@ -2662,13 +2644,13 @@
         <v>31</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="D33" s="9" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="E33" s="9" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="F33" s="1"/>
     </row>
@@ -2680,13 +2662,13 @@
         <v>31</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="D34" s="9" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="E34" s="9" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="F34" s="1"/>
     </row>
@@ -2698,13 +2680,13 @@
         <v>31</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="D35" s="9" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="E35" s="9" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="F35" s="1"/>
     </row>
@@ -2716,13 +2698,13 @@
         <v>8</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="D36" s="9" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="E36" s="9" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="F36" s="1"/>
     </row>
@@ -2734,13 +2716,13 @@
         <v>8</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="D37" s="9" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="E37" s="9" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="F37" s="1"/>
     </row>
@@ -2752,13 +2734,13 @@
         <v>6</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="D38" s="9" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="E38" s="9" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="F38" s="1"/>
     </row>
@@ -2770,13 +2752,13 @@
         <v>8</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="D39" s="9" t="s">
+        <v>260</v>
+      </c>
+      <c r="E39" s="9" t="s">
         <v>258</v>
-      </c>
-      <c r="E39" s="9" t="s">
-        <v>256</v>
       </c>
       <c r="F39" s="1"/>
     </row>
@@ -2788,13 +2770,13 @@
         <v>15</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="D40" s="9" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="E40" s="9" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="F40" s="1"/>
     </row>
@@ -2806,13 +2788,13 @@
         <v>6</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="D41" s="9" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="E41" s="9" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="F41" s="1"/>
     </row>
@@ -2824,13 +2806,13 @@
         <v>6</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="D42" s="9" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="E42" s="9" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="F42" s="1"/>
     </row>
@@ -2842,13 +2824,13 @@
         <v>8</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="D43" s="9" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="E43" s="9" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="F43" s="1"/>
     </row>
@@ -2860,13 +2842,13 @@
         <v>8</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="D44" s="9" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="E44" s="9" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="F44" s="1"/>
     </row>
@@ -2878,13 +2860,13 @@
         <v>8</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="D45" s="9" t="s">
+        <v>260</v>
+      </c>
+      <c r="E45" s="9" t="s">
         <v>258</v>
-      </c>
-      <c r="E45" s="9" t="s">
-        <v>256</v>
       </c>
       <c r="F45" s="1"/>
     </row>
@@ -2896,13 +2878,13 @@
         <v>6</v>
       </c>
       <c r="C46" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="D46" s="9" t="s">
         <v>281</v>
       </c>
-      <c r="D46" s="9" t="s">
+      <c r="E46" s="9" t="s">
         <v>279</v>
-      </c>
-      <c r="E46" s="9" t="s">
-        <v>277</v>
       </c>
       <c r="F46" s="1"/>
     </row>
@@ -2914,13 +2896,13 @@
         <v>8</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="D47" s="9" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="E47" s="9" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="F47" s="1"/>
     </row>
@@ -2932,13 +2914,13 @@
         <v>8</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="D48" s="9" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="E48" s="9" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="F48" s="1"/>
     </row>
@@ -2950,13 +2932,13 @@
         <v>6</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="D49" s="9" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="E49" s="9" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="F49" s="1"/>
     </row>
@@ -2968,13 +2950,13 @@
         <v>8</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="D50" s="9" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="E50" s="9" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="F50" s="1"/>
     </row>
@@ -2986,13 +2968,13 @@
         <v>6</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="D51" s="9" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="E51" s="9" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="F51" s="1"/>
     </row>
@@ -3004,13 +2986,13 @@
         <v>8</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="D52" s="9" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="E52" s="9" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="F52" s="1"/>
     </row>
@@ -3022,13 +3004,13 @@
         <v>6</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="D53" s="9" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="E53" s="9" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="F53" s="1"/>
     </row>
@@ -3040,13 +3022,13 @@
         <v>15</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="D54" s="9" t="s">
+        <v>274</v>
+      </c>
+      <c r="E54" s="9" t="s">
         <v>272</v>
-      </c>
-      <c r="E54" s="9" t="s">
-        <v>270</v>
       </c>
       <c r="F54" s="1"/>
     </row>
@@ -3058,13 +3040,13 @@
         <v>31</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="D55" s="9" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="E55" s="9" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="F55" s="1"/>
     </row>
@@ -3076,13 +3058,13 @@
         <v>33</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="D56" s="9" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="E56" s="9" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="F56" s="1"/>
     </row>
@@ -3094,13 +3076,13 @@
         <v>6</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="D57" s="9" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="E57" s="9" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="F57" s="1"/>
     </row>
@@ -3112,13 +3094,13 @@
         <v>36</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="D58" s="9" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="E58" s="9" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="F58" s="1"/>
     </row>
@@ -3130,13 +3112,13 @@
         <v>36</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="D59" s="9" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="E59" s="9" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="F59" s="1"/>
     </row>
@@ -3148,13 +3130,13 @@
         <v>15</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="D60" s="9" t="s">
+        <v>274</v>
+      </c>
+      <c r="E60" s="9" t="s">
         <v>272</v>
-      </c>
-      <c r="E60" s="9" t="s">
-        <v>270</v>
       </c>
       <c r="F60" s="1"/>
     </row>
@@ -3166,13 +3148,13 @@
         <v>15</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="D61" s="9" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="E61" s="9" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="F61" s="1"/>
     </row>
@@ -3184,13 +3166,13 @@
         <v>31</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="D62" s="9" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="E62" s="9" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="F62" s="1"/>
     </row>
@@ -3202,13 +3184,13 @@
         <v>31</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="D63" s="9" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="E63" s="9" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="F63" s="1"/>
     </row>
@@ -3220,13 +3202,13 @@
         <v>31</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="D64" s="9" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="E64" s="9" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="F64" s="1"/>
     </row>
@@ -3238,13 +3220,13 @@
         <v>31</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="D65" s="9" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="E65" s="9" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="F65" s="1"/>
     </row>
@@ -3253,16 +3235,16 @@
         <v>74</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="D66" s="9" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="E66" s="9" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="F66" s="1"/>
     </row>
@@ -3271,179 +3253,195 @@
         <v>75</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="C67" s="2" t="s">
         <v>167</v>
       </c>
       <c r="D67" s="9" t="s">
-        <v>219</v>
-      </c>
-      <c r="E67" s="15" t="s">
-        <v>284</v>
-      </c>
-      <c r="F67" s="3"/>
+        <v>221</v>
+      </c>
+      <c r="E67" s="10"/>
+      <c r="F67" s="3" t="s">
+        <v>187</v>
+      </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A68" s="1" t="s">
         <v>76</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="C68" s="2" t="s">
         <v>167</v>
       </c>
       <c r="D68" s="9" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="E68" s="9" t="s">
-        <v>206</v>
-      </c>
-      <c r="F68" s="4"/>
+        <v>207</v>
+      </c>
+      <c r="F68" s="4" t="s">
+        <v>187</v>
+      </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A69" s="1" t="s">
         <v>77</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="D69" s="9" t="s">
+        <v>212</v>
+      </c>
+      <c r="E69" s="9" t="s">
         <v>210</v>
       </c>
-      <c r="E69" s="9" t="s">
-        <v>208</v>
-      </c>
-      <c r="F69" s="4"/>
+      <c r="F69" s="4" t="s">
+        <v>187</v>
+      </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A70" s="1" t="s">
         <v>78</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C70" s="2" t="s">
         <v>167</v>
       </c>
       <c r="D70" s="9" t="s">
+        <v>211</v>
+      </c>
+      <c r="E70" s="9" t="s">
         <v>209</v>
       </c>
-      <c r="E70" s="9" t="s">
-        <v>283</v>
-      </c>
-      <c r="F70" s="4"/>
+      <c r="F70" s="4" t="s">
+        <v>187</v>
+      </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A71" s="1" t="s">
         <v>79</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="C71" s="2" t="s">
         <v>167</v>
       </c>
       <c r="D71" s="9" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="E71" s="9" t="s">
-        <v>205</v>
-      </c>
-      <c r="F71" s="4"/>
+        <v>206</v>
+      </c>
+      <c r="F71" s="4" t="s">
+        <v>187</v>
+      </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A72" s="1" t="s">
         <v>80</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="D72" s="9" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="E72" s="9" t="s">
-        <v>205</v>
-      </c>
-      <c r="F72" s="4"/>
+        <v>206</v>
+      </c>
+      <c r="F72" s="4" t="s">
+        <v>187</v>
+      </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A73" s="1" t="s">
         <v>81</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="D73" s="9" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="E73" s="9" t="s">
-        <v>208</v>
-      </c>
-      <c r="F73" s="4"/>
+        <v>210</v>
+      </c>
+      <c r="F73" s="4" t="s">
+        <v>187</v>
+      </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A74" s="1" t="s">
         <v>82</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C74" s="2" t="s">
         <v>167</v>
       </c>
       <c r="D74" s="9" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="E74" s="9" t="s">
-        <v>207</v>
-      </c>
-      <c r="F74" s="4"/>
+        <v>208</v>
+      </c>
+      <c r="F74" s="4" t="s">
+        <v>187</v>
+      </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A75" s="1" t="s">
         <v>83</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="C75" s="2" t="s">
         <v>167</v>
       </c>
       <c r="D75" s="9" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="E75" s="9" t="s">
-        <v>206</v>
-      </c>
-      <c r="F75" s="4"/>
+        <v>207</v>
+      </c>
+      <c r="F75" s="4" t="s">
+        <v>187</v>
+      </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A76" s="1" t="s">
         <v>84</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="C76" s="2" t="s">
         <v>167</v>
       </c>
       <c r="D76" s="9" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="E76" s="10"/>
       <c r="F76" s="4" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.4">
@@ -3451,17 +3449,17 @@
         <v>85</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="D77" s="9" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="E77" s="11"/>
       <c r="F77" s="4" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.4">
@@ -3469,17 +3467,17 @@
         <v>86</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="C78" s="2" t="s">
         <v>167</v>
       </c>
       <c r="D78" s="9" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="E78" s="11"/>
       <c r="F78" s="4" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.4">
@@ -3487,16 +3485,16 @@
         <v>87</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="C79" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="D79" s="9" t="s">
         <v>232</v>
       </c>
-      <c r="D79" s="9" t="s">
-        <v>230</v>
-      </c>
       <c r="E79" s="12" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="F79" s="1"/>
     </row>
@@ -3505,16 +3503,16 @@
         <v>88</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="D80" s="9" t="s">
+        <v>232</v>
+      </c>
+      <c r="E80" s="9" t="s">
         <v>230</v>
-      </c>
-      <c r="E80" s="9" t="s">
-        <v>228</v>
       </c>
       <c r="F80" s="1"/>
     </row>
@@ -3523,16 +3521,16 @@
         <v>89</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="C81" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="D81" s="9" t="s">
         <v>233</v>
       </c>
-      <c r="D81" s="9" t="s">
-        <v>231</v>
-      </c>
       <c r="E81" s="9" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="F81" s="1"/>
     </row>
@@ -3541,16 +3539,16 @@
         <v>90</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="D82" s="9" t="s">
+        <v>232</v>
+      </c>
+      <c r="E82" s="9" t="s">
         <v>230</v>
-      </c>
-      <c r="E82" s="9" t="s">
-        <v>228</v>
       </c>
       <c r="F82" s="1"/>
     </row>
@@ -3559,16 +3557,16 @@
         <v>91</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="C83" s="2">
         <v>3216</v>
       </c>
       <c r="D83" s="9" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="E83" s="9" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="F83" s="1"/>
     </row>
@@ -3577,16 +3575,16 @@
         <v>92</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="C84" s="2">
         <v>3216</v>
       </c>
       <c r="D84" s="9" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="E84" s="9" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="F84" s="1"/>
     </row>
@@ -3598,13 +3596,13 @@
         <v>94</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="D85" s="9" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="E85" s="9" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="F85" s="1"/>
     </row>
@@ -3616,13 +3614,13 @@
         <v>562</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="D86" s="9" t="s">
+        <v>256</v>
+      </c>
+      <c r="E86" s="9" t="s">
         <v>254</v>
-      </c>
-      <c r="E86" s="9" t="s">
-        <v>252</v>
       </c>
       <c r="F86" s="1"/>
     </row>
@@ -3634,13 +3632,13 @@
         <v>97</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="D87" s="9" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="E87" s="9" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="F87" s="1"/>
     </row>
@@ -3652,13 +3650,13 @@
         <v>99</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="D88" s="9" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="E88" s="9" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="F88" s="1"/>
     </row>
@@ -3670,13 +3668,13 @@
         <v>101</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="D89" s="9" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="E89" s="9" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="F89" s="1"/>
     </row>
@@ -3688,13 +3686,13 @@
         <v>103</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="D90" s="9" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="E90" s="9" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="F90" s="1"/>
     </row>
@@ -3706,13 +3704,13 @@
         <v>101</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="D91" s="9" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="E91" s="9" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="F91" s="1"/>
     </row>
@@ -3724,13 +3722,13 @@
         <v>103</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="D92" s="9" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="E92" s="13" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="F92" s="1"/>
     </row>
@@ -3742,13 +3740,13 @@
         <v>101</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="D93" s="9" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="E93" s="9" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="F93" s="1"/>
     </row>
@@ -3760,13 +3758,13 @@
         <v>108</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="D94" s="9" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="E94" s="9" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="F94" s="1"/>
     </row>
@@ -3778,13 +3776,13 @@
         <v>108</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="D95" s="9" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="E95" s="9" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="F95" s="1"/>
     </row>
@@ -3796,13 +3794,13 @@
         <v>111</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="D96" s="9" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="E96" s="9" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="F96" s="1"/>
     </row>
@@ -3814,13 +3812,13 @@
         <v>475</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="D97" s="9" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="E97" s="9" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="F97" s="1"/>
     </row>
@@ -3832,13 +3830,13 @@
         <v>101</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="D98" s="9" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="E98" s="9" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="F98" s="1"/>
     </row>
@@ -3850,13 +3848,13 @@
         <v>108</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="D99" s="9" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="E99" s="9" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="F99" s="1"/>
     </row>
@@ -3868,13 +3866,13 @@
         <v>108</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="D100" s="9" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="E100" s="9" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="F100" s="1"/>
     </row>
@@ -3886,13 +3884,13 @@
         <v>108</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="D101" s="9" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="E101" s="9" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="F101" s="1"/>
     </row>
@@ -3904,13 +3902,13 @@
         <v>108</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="D102" s="9" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="E102" s="9" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="F102" s="1"/>
     </row>
@@ -3922,13 +3920,13 @@
         <v>99</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="D103" s="9" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="E103" s="9" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="F103" s="1"/>
     </row>
@@ -3940,13 +3938,13 @@
         <v>99</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="D104" s="9" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="E104" s="9" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="F104" s="1"/>
     </row>
@@ -3958,13 +3956,13 @@
         <v>99</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="D105" s="9" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="E105" s="9" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="F105" s="1"/>
     </row>
@@ -3976,13 +3974,13 @@
         <v>99</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="D106" s="9" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="E106" s="9" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="F106" s="1"/>
     </row>
@@ -3994,13 +3992,13 @@
         <v>0</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="D107" s="9" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="E107" s="9" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="F107" s="1"/>
     </row>
@@ -4012,13 +4010,13 @@
         <v>97</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="D108" s="9" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="E108" s="9" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="F108" s="1"/>
     </row>
@@ -4030,13 +4028,13 @@
         <v>101</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="D109" s="9" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="E109" s="9" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="F109" s="1"/>
     </row>
@@ -4048,13 +4046,13 @@
         <v>103</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="D110" s="9" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="E110" s="9" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="F110" s="1"/>
     </row>
@@ -4066,13 +4064,13 @@
         <v>101</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="D111" s="9" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="E111" s="9" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="F111" s="1"/>
     </row>
@@ -4084,13 +4082,13 @@
         <v>103</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="D112" s="9" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="E112" s="9" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="F112" s="1"/>
     </row>
@@ -4102,13 +4100,13 @@
         <v>101</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="D113" s="9" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="E113" s="9" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="F113" s="1"/>
     </row>
@@ -4120,13 +4118,13 @@
         <v>108</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="D114" s="9" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="E114" s="9" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="F114" s="1"/>
     </row>
@@ -4138,13 +4136,13 @@
         <v>108</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="D115" s="9" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="E115" s="9" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="F115" s="1"/>
     </row>
@@ -4156,13 +4154,13 @@
         <v>111</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="D116" s="9" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="E116" s="9" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="F116" s="1"/>
     </row>
@@ -4174,13 +4172,13 @@
         <v>475</v>
       </c>
       <c r="C117" s="2" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="D117" s="9" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="E117" s="9" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="F117" s="1"/>
     </row>
@@ -4192,13 +4190,13 @@
         <v>101</v>
       </c>
       <c r="C118" s="2" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="D118" s="9" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="E118" s="9" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="F118" s="1"/>
     </row>
@@ -4210,13 +4208,13 @@
         <v>108</v>
       </c>
       <c r="C119" s="2" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="D119" s="9" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="E119" s="9" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="F119" s="1"/>
     </row>
@@ -4228,13 +4226,13 @@
         <v>108</v>
       </c>
       <c r="C120" s="2" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="D120" s="9" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="E120" s="9" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="F120" s="1"/>
     </row>
@@ -4246,13 +4244,13 @@
         <v>108</v>
       </c>
       <c r="C121" s="2" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="D121" s="9" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="E121" s="9" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="F121" s="1"/>
     </row>
@@ -4264,13 +4262,13 @@
         <v>108</v>
       </c>
       <c r="C122" s="2" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="D122" s="9" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="E122" s="9" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="F122" s="1"/>
     </row>
@@ -4282,13 +4280,13 @@
         <v>99</v>
       </c>
       <c r="C123" s="2" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="D123" s="9" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="E123" s="9" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="F123" s="1"/>
     </row>
@@ -4300,13 +4298,13 @@
         <v>99</v>
       </c>
       <c r="C124" s="2" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="D124" s="9" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="E124" s="9" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="F124" s="1"/>
     </row>
@@ -4318,13 +4316,13 @@
         <v>99</v>
       </c>
       <c r="C125" s="2" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="D125" s="9" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="E125" s="9" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="F125" s="1"/>
     </row>
@@ -4336,13 +4334,13 @@
         <v>99</v>
       </c>
       <c r="C126" s="2" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="D126" s="9" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="E126" s="9" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="F126" s="1"/>
     </row>
@@ -4354,13 +4352,13 @@
         <v>562</v>
       </c>
       <c r="C127" s="2" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="D127" s="9" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="E127" s="9" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="F127" s="1"/>
     </row>
@@ -4380,7 +4378,9 @@
       <c r="E128" s="9" t="s">
         <v>172</v>
       </c>
-      <c r="F128" s="4"/>
+      <c r="F128" s="4" t="s">
+        <v>187</v>
+      </c>
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A129" s="1" t="s">
@@ -4396,26 +4396,28 @@
         <v>166</v>
       </c>
       <c r="E129" s="9" t="s">
-        <v>285</v>
-      </c>
-      <c r="F129" s="4"/>
+        <v>172</v>
+      </c>
+      <c r="F129" s="4" t="s">
+        <v>187</v>
+      </c>
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A130" s="1" t="s">
         <v>145</v>
       </c>
       <c r="B130" s="2" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="C130" s="2" t="s">
         <v>167</v>
       </c>
       <c r="D130" s="9" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="E130" s="10"/>
       <c r="F130" s="4" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.4">
@@ -4423,17 +4425,17 @@
         <v>146</v>
       </c>
       <c r="B131" s="2" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="C131" s="2" t="s">
         <v>167</v>
       </c>
       <c r="D131" s="9" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="E131" s="11"/>
       <c r="F131" s="4" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.4">
@@ -4452,7 +4454,9 @@
       <c r="E132" s="9" t="s">
         <v>168</v>
       </c>
-      <c r="F132" s="4"/>
+      <c r="F132" s="4" t="s">
+        <v>187</v>
+      </c>
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A133" s="1" t="s">
@@ -4470,7 +4474,9 @@
       <c r="E133" s="9" t="s">
         <v>169</v>
       </c>
-      <c r="F133" s="4"/>
+      <c r="F133" s="4" t="s">
+        <v>187</v>
+      </c>
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A134" s="1" t="s">
@@ -4513,16 +4519,16 @@
         <v>152</v>
       </c>
       <c r="B136" s="2" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="C136" s="2" t="s">
         <v>153</v>
       </c>
       <c r="D136" s="9" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="E136" s="9" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="F136" s="1"/>
     </row>
@@ -4531,16 +4537,16 @@
         <v>154</v>
       </c>
       <c r="B137" s="2" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="C137" s="2" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="D137" s="9" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="E137" s="9" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="F137" s="1"/>
     </row>
@@ -4549,16 +4555,16 @@
         <v>155</v>
       </c>
       <c r="B138" s="2" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="C138" s="2" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="D138" s="9" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="E138" s="9" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="F138" s="1"/>
     </row>
@@ -4567,16 +4573,16 @@
         <v>156</v>
       </c>
       <c r="B139" s="2" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="C139" s="2" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="D139" s="9" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="E139" s="9" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="F139" s="1"/>
     </row>
@@ -4585,18 +4591,20 @@
         <v>157</v>
       </c>
       <c r="B140" s="2" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="C140" s="2" t="s">
         <v>167</v>
       </c>
       <c r="D140" s="9" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="E140" s="9" t="s">
-        <v>181</v>
-      </c>
-      <c r="F140" s="3"/>
+        <v>182</v>
+      </c>
+      <c r="F140" s="3" t="s">
+        <v>187</v>
+      </c>
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A141" s="1" t="s">
@@ -4606,15 +4614,17 @@
         <v>159</v>
       </c>
       <c r="C141" s="2" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="D141" s="9" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="E141" s="9" t="s">
-        <v>182</v>
-      </c>
-      <c r="F141" s="4"/>
+        <v>183</v>
+      </c>
+      <c r="F141" s="4" t="s">
+        <v>187</v>
+      </c>
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A142" s="5" t="s">
@@ -4627,10 +4637,10 @@
         <v>177</v>
       </c>
       <c r="D142" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="E142" s="14" t="s">
         <v>178</v>
-      </c>
-      <c r="E142" s="14" t="s">
-        <v>286</v>
       </c>
       <c r="F142" s="5"/>
     </row>

</xml_diff>